<commit_message>
test vector gen for 3388
</commit_message>
<xml_diff>
--- a/MeasurementParameters.xlsx
+++ b/MeasurementParameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\meas\p3388_tigwelding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\meas\p3388_tigwelding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5498E62D-4AFD-46C9-AE24-76C963EC5382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B986BC02-B12B-463C-93CF-87768BA5CA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21375" yWindow="4965" windowWidth="21330" windowHeight="15915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_catalog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="81">
   <si>
     <t>arc length may be suggested by different weld metal. 
 The distance between antenna and welding table : 9 feet to the first edge, another 4 feet to the other edge. 
@@ -259,6 +259,30 @@
   <si>
     <t xml:space="preserve">combined cable insertion loss (cables 4+5) : 10.31 dbm (test with -10dbm signal and 20 db attenuator)
 insertion loss from non-calibrated VNA : 6.55db for cable 1,  10.78 for cable 2,   10.49  for cable 3,   7.92 for cable 4,  5.4 for cable 5,  4.07 for cable 6   </t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>baseline_2.4GHz_IQ_time.iq</t>
+  </si>
+  <si>
+    <t>baseline_5.3GHz_IQ_time.iq</t>
+  </si>
+  <si>
+    <t>baseline_0301_5GHz_IQ_time.iq</t>
+  </si>
+  <si>
+    <t>baseline_0301_24GHz_IQ_time.iq</t>
+  </si>
+  <si>
+    <t>baseline_0301_900_IQ_time.iq</t>
+  </si>
+  <si>
+    <t>baseline measurement</t>
+  </si>
+  <si>
+    <t>BASELINE</t>
   </si>
 </sst>
 </file>
@@ -337,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -375,6 +399,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -384,6 +411,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,52 +726,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
     </row>
     <row r="2" spans="1:20" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
@@ -2682,6 +2715,321 @@
         <v>60</v>
       </c>
       <c r="T34" s="15"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="8">
+        <v>100</v>
+      </c>
+      <c r="C35" s="8">
+        <v>1</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="26">
+        <v>0</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35" s="8">
+        <v>0</v>
+      </c>
+      <c r="J35" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M35" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="N35" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="O35" s="28">
+        <v>0</v>
+      </c>
+      <c r="P35" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="28">
+        <v>4</v>
+      </c>
+      <c r="R35" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="S35" t="s">
+        <v>74</v>
+      </c>
+      <c r="T35" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="8">
+        <v>100</v>
+      </c>
+      <c r="C36" s="8">
+        <v>2</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="26">
+        <v>0</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I36" s="8">
+        <v>0</v>
+      </c>
+      <c r="J36" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L36" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="N36" s="28">
+        <v>5.3</v>
+      </c>
+      <c r="O36" s="28">
+        <v>0</v>
+      </c>
+      <c r="P36" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="28">
+        <v>4</v>
+      </c>
+      <c r="R36" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="S36" t="s">
+        <v>75</v>
+      </c>
+      <c r="T36" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="8">
+        <v>100</v>
+      </c>
+      <c r="C37" s="8">
+        <v>3</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="26">
+        <v>0</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I37" s="8">
+        <v>0</v>
+      </c>
+      <c r="J37" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L37" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M37" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="N37" s="28">
+        <v>5.3</v>
+      </c>
+      <c r="O37" s="28">
+        <v>0</v>
+      </c>
+      <c r="P37" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="28">
+        <v>4</v>
+      </c>
+      <c r="R37" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="S37" t="s">
+        <v>76</v>
+      </c>
+      <c r="T37" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="8">
+        <v>100</v>
+      </c>
+      <c r="C38" s="8">
+        <v>4</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="26">
+        <v>0</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I38" s="8">
+        <v>0</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L38" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M38" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="N38" s="28">
+        <v>2.4</v>
+      </c>
+      <c r="O38" s="28">
+        <v>0</v>
+      </c>
+      <c r="P38" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="28">
+        <v>4</v>
+      </c>
+      <c r="R38" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="S38" t="s">
+        <v>77</v>
+      </c>
+      <c r="T38" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="8">
+        <v>100</v>
+      </c>
+      <c r="C39" s="8">
+        <v>5</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="26">
+        <v>0</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I39" s="8">
+        <v>0</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="L39" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M39" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="N39" s="28">
+        <v>0.9</v>
+      </c>
+      <c r="O39" s="28">
+        <v>0</v>
+      </c>
+      <c r="P39" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="28">
+        <v>4</v>
+      </c>
+      <c r="R39" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="S39" t="s">
+        <v>78</v>
+      </c>
+      <c r="T39" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="25"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2694,6 +3042,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -2704,15 +3061,6 @@
     <TaxCatchAll xmlns="24df8fc7-eba8-42a4-b5bf-4369c8aae6a7" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2993,6 +3341,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D522714-B2F9-49FA-830F-9865B4DCB893}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15746BA2-8216-4C14-95EB-B5AE0BF64B68}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3000,14 +3356,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="80d50089-c5c1-405f-b8e5-a46763c1f187"/>
     <ds:schemaRef ds:uri="24df8fc7-eba8-42a4-b5bf-4369c8aae6a7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D522714-B2F9-49FA-830F-9865B4DCB893}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
clean up test vector generation
</commit_message>
<xml_diff>
--- a/MeasurementParameters.xlsx
+++ b/MeasurementParameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\meas\p3388_tigwelding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B986BC02-B12B-463C-93CF-87768BA5CA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9AD537-B237-4A66-9131-70B563F1CD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21375" yWindow="4965" windowWidth="21330" windowHeight="15915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_catalog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="82">
   <si>
     <t>arc length may be suggested by different weld metal. 
 The distance between antenna and welding table : 9 feet to the first edge, another 4 feet to the other edge. 
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>BASELINE</t>
+  </si>
+  <si>
+    <t>Capture is same as previous</t>
   </si>
 </sst>
 </file>
@@ -401,6 +404,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -411,12 +420,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,7 +703,7 @@
   <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,52 +729,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
     </row>
     <row r="2" spans="1:20" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
     </row>
     <row r="3" spans="1:20" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
@@ -992,6 +995,9 @@
       <c r="S6" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="T6" s="14" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
@@ -2717,7 +2723,7 @@
       <c r="T34" s="15"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="21" t="s">
         <v>80</v>
       </c>
       <c r="B35" s="8">
@@ -2726,49 +2732,49 @@
       <c r="C35" s="8">
         <v>1</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="26">
+      <c r="E35" s="22">
         <v>0</v>
       </c>
-      <c r="F35" s="25" t="s">
+      <c r="F35" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="G35" s="25" t="s">
+      <c r="G35" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="H35" s="25" t="s">
+      <c r="H35" s="21" t="s">
         <v>43</v>
       </c>
       <c r="I35" s="8">
         <v>0</v>
       </c>
-      <c r="J35" s="25" t="s">
+      <c r="J35" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="K35" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="L35" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="M35" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="N35" s="28">
+      <c r="K35" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M35" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N35" s="24">
         <v>2.5</v>
       </c>
-      <c r="O35" s="28">
+      <c r="O35" s="24">
         <v>0</v>
       </c>
-      <c r="P35" s="28">
+      <c r="P35" s="24">
         <v>0</v>
       </c>
-      <c r="Q35" s="28">
+      <c r="Q35" s="24">
         <v>4</v>
       </c>
-      <c r="R35" s="25" t="s">
+      <c r="R35" s="21" t="s">
         <v>74</v>
       </c>
       <c r="S35" t="s">
@@ -2779,7 +2785,7 @@
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="21" t="s">
         <v>80</v>
       </c>
       <c r="B36" s="8">
@@ -2788,49 +2794,49 @@
       <c r="C36" s="8">
         <v>2</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="26">
+      <c r="E36" s="22">
         <v>0</v>
       </c>
-      <c r="F36" s="25" t="s">
+      <c r="F36" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="G36" s="25" t="s">
+      <c r="G36" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="21" t="s">
         <v>43</v>
       </c>
       <c r="I36" s="8">
         <v>0</v>
       </c>
-      <c r="J36" s="25" t="s">
+      <c r="J36" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="K36" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="L36" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="N36" s="28">
+      <c r="K36" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L36" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N36" s="24">
         <v>5.3</v>
       </c>
-      <c r="O36" s="28">
+      <c r="O36" s="24">
         <v>0</v>
       </c>
-      <c r="P36" s="28">
+      <c r="P36" s="24">
         <v>0</v>
       </c>
-      <c r="Q36" s="28">
+      <c r="Q36" s="24">
         <v>4</v>
       </c>
-      <c r="R36" s="25" t="s">
+      <c r="R36" s="21" t="s">
         <v>75</v>
       </c>
       <c r="S36" t="s">
@@ -2841,7 +2847,7 @@
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="21" t="s">
         <v>80</v>
       </c>
       <c r="B37" s="8">
@@ -2850,49 +2856,49 @@
       <c r="C37" s="8">
         <v>3</v>
       </c>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E37" s="26">
+      <c r="E37" s="22">
         <v>0</v>
       </c>
-      <c r="F37" s="25" t="s">
+      <c r="F37" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="G37" s="25" t="s">
+      <c r="G37" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="H37" s="25" t="s">
+      <c r="H37" s="21" t="s">
         <v>43</v>
       </c>
       <c r="I37" s="8">
         <v>0</v>
       </c>
-      <c r="J37" s="25" t="s">
+      <c r="J37" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="K37" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="L37" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="M37" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="N37" s="28">
+      <c r="K37" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L37" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M37" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N37" s="24">
         <v>5.3</v>
       </c>
-      <c r="O37" s="28">
+      <c r="O37" s="24">
         <v>0</v>
       </c>
-      <c r="P37" s="28">
+      <c r="P37" s="24">
         <v>0</v>
       </c>
-      <c r="Q37" s="28">
+      <c r="Q37" s="24">
         <v>4</v>
       </c>
-      <c r="R37" s="25" t="s">
+      <c r="R37" s="21" t="s">
         <v>76</v>
       </c>
       <c r="S37" t="s">
@@ -2903,7 +2909,7 @@
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="21" t="s">
         <v>80</v>
       </c>
       <c r="B38" s="8">
@@ -2912,49 +2918,49 @@
       <c r="C38" s="8">
         <v>4</v>
       </c>
-      <c r="D38" s="25" t="s">
+      <c r="D38" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E38" s="26">
+      <c r="E38" s="22">
         <v>0</v>
       </c>
-      <c r="F38" s="25" t="s">
+      <c r="F38" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="G38" s="25" t="s">
+      <c r="G38" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="H38" s="25" t="s">
+      <c r="H38" s="21" t="s">
         <v>43</v>
       </c>
       <c r="I38" s="8">
         <v>0</v>
       </c>
-      <c r="J38" s="25" t="s">
+      <c r="J38" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="K38" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="L38" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="M38" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="N38" s="28">
+      <c r="K38" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L38" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M38" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N38" s="24">
         <v>2.4</v>
       </c>
-      <c r="O38" s="28">
+      <c r="O38" s="24">
         <v>0</v>
       </c>
-      <c r="P38" s="28">
+      <c r="P38" s="24">
         <v>0</v>
       </c>
-      <c r="Q38" s="28">
+      <c r="Q38" s="24">
         <v>4</v>
       </c>
-      <c r="R38" s="25" t="s">
+      <c r="R38" s="21" t="s">
         <v>77</v>
       </c>
       <c r="S38" t="s">
@@ -2965,7 +2971,7 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="21" t="s">
         <v>80</v>
       </c>
       <c r="B39" s="8">
@@ -2974,49 +2980,49 @@
       <c r="C39" s="8">
         <v>5</v>
       </c>
-      <c r="D39" s="25" t="s">
+      <c r="D39" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E39" s="26">
+      <c r="E39" s="22">
         <v>0</v>
       </c>
-      <c r="F39" s="25" t="s">
+      <c r="F39" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="G39" s="25" t="s">
+      <c r="G39" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="H39" s="25" t="s">
+      <c r="H39" s="21" t="s">
         <v>43</v>
       </c>
       <c r="I39" s="8">
         <v>0</v>
       </c>
-      <c r="J39" s="25" t="s">
+      <c r="J39" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="K39" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="L39" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="M39" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="N39" s="28">
+      <c r="K39" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L39" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M39" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N39" s="24">
         <v>0.9</v>
       </c>
-      <c r="O39" s="28">
+      <c r="O39" s="24">
         <v>0</v>
       </c>
-      <c r="P39" s="28">
+      <c r="P39" s="24">
         <v>0</v>
       </c>
-      <c r="Q39" s="28">
+      <c r="Q39" s="24">
         <v>4</v>
       </c>
-      <c r="R39" s="25" t="s">
+      <c r="R39" s="21" t="s">
         <v>78</v>
       </c>
       <c r="S39" t="s">
@@ -3027,7 +3033,7 @@
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
     </row>
@@ -3042,15 +3048,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -3061,6 +3058,15 @@
     <TaxCatchAll xmlns="24df8fc7-eba8-42a4-b5bf-4369c8aae6a7" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3341,14 +3347,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D522714-B2F9-49FA-830F-9865B4DCB893}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15746BA2-8216-4C14-95EB-B5AE0BF64B68}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3356,6 +3354,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="80d50089-c5c1-405f-b8e5-a46763c1f187"/>
     <ds:schemaRef ds:uri="24df8fc7-eba8-42a4-b5bf-4369c8aae6a7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D522714-B2F9-49FA-830F-9865B4DCB893}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>